<commit_message>
add embedded plot example
</commit_message>
<xml_diff>
--- a/matplotlib/matplotlib.xlsx
+++ b/matplotlib/matplotlib.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\pyxll-examples\matplotlib\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="6810" windowHeight="5040"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>FIGNAME</t>
   </si>
@@ -39,6 +34,9 @@
   </si>
   <si>
     <t>ewma</t>
+  </si>
+  <si>
+    <t>Embedded Plot</t>
   </si>
 </sst>
 </file>
@@ -178,6 +176,49 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1323975</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="ewma"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:link="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4238625" y="1781175"/>
+          <a:ext cx="5391150" cy="4043363"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -221,7 +262,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,7 +297,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,7 +506,8 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C359"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B3:F359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,37 +516,56 @@
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>_xll.mpl_plot_ewma(C6,B10:B359,C10:C359,C7)</f>
         <v>[Plotted 'ewma']</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="str">
+        <f>_xll.mpl_plot_ewma_embedded(F6,B10:B359,C10:C359,F7)</f>
+        <v>[Plotted 'ewma']</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
@@ -512,7 +573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>0</v>
       </c>
@@ -521,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f>B10+0.05</f>
         <v>0.05</v>
@@ -531,7 +592,7 @@
         <v>7.2798500044011921E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <f t="shared" ref="B12:B75" si="1">B11+0.05</f>
         <v>0.1</v>
@@ -541,7 +602,7 @@
         <v>0.30260644336050269</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
@@ -551,7 +612,7 @@
         <v>0.5748347242212053</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <f t="shared" si="1"/>
         <v>0.2</v>
@@ -561,7 +622,7 @@
         <v>0.63218922317423532</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -571,7 +632,7 @@
         <v>0.42798728108473139</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <f t="shared" si="1"/>
         <v>0.3</v>
@@ -4014,11 +4075,13 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4031,9 +4094,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Use Shapes.AddPicture instead of Pictures.Insert. This allows the image to be saved as part of the Excel file instead of referencing the image file.
</commit_message>
<xml_diff>
--- a/matplotlib/matplotlib.xlsx
+++ b/matplotlib/matplotlib.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -180,34 +180,40 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1323975</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="ewma"/>
+        <xdr:cNvPr id="5" name="ewma"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:link="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4238625" y="1781175"/>
-          <a:ext cx="5391150" cy="4043363"/>
+          <a:off x="4276725" y="1781175"/>
+          <a:ext cx="5048250" cy="3786188"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
Switch matplotlib examples to use PySide6
And add a function to display and update a matplotlib CTP from an Excel
worksheet function.
</commit_message>
<xml_diff>
--- a/matplotlib/matplotlib.xlsx
+++ b/matplotlib/matplotlib.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\pyxll-examples\matplotlib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CAB574-D0DD-4073-AFFE-9A895D1F83B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4AC70A-54F2-4FA8-B6DA-0F8899958DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8920" yWindow="3370" windowWidth="24210" windowHeight="15610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="1440" windowWidth="28320" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +38,21 @@
     <author>Tony Roberts</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{CAA0A6B3-9E8F-4D5F-A322-4781AE96BA59}">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{E155C052-BAD6-4E27-A968-6DD17F1058D4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Update SPAN to see the chart update</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{CAA0A6B3-9E8F-4D5F-A322-4781AE96BA59}">
       <text>
         <r>
           <rPr>
@@ -53,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{E155C052-BAD6-4E27-A968-6DD17F1058D4}">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{93A1809D-9697-4515-B71D-982E79A832B6}">
       <text>
         <r>
           <rPr>
@@ -63,7 +76,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Update SPAN to see the chart update</t>
+          <t>Set this to TRUE to show the plot in a separate window</t>
         </r>
       </text>
     </comment>
@@ -94,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>X</t>
   </si>
@@ -106,6 +119,9 @@
   </si>
   <si>
     <t>Matplotlib Example</t>
+  </si>
+  <si>
+    <t>ENABLE CTP</t>
   </si>
 </sst>
 </file>
@@ -257,22 +273,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1270000</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>166370</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="_PYPLOT_B4">
+        <xdr:cNvPr id="36" name="_PYPLOT_D5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE6DFCA8-6BCB-6ACE-07A7-19C0D66667F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10CD0F11-D360-BD4F-3927-9819BE4B029F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -294,7 +310,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5708650" y="774700"/>
+          <a:off x="4794250" y="1352550"/>
           <a:ext cx="5852160" cy="4389120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -595,7 +611,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:C358"/>
+  <dimension ref="B2:D358"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -607,26 +623,36 @@
     <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B4" s="3" t="str" cm="1">
-        <f t="array" ref="B4">_xll.mpl_plot_ewma(B9:B358,C9:C358,C6)</f>
-        <v>Figure@16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6">
+        <v>100</v>
+      </c>
+      <c r="D5" s="3" t="str" cm="1">
+        <f t="array" ref="D5">_xll.mpl_plot_ewma(B9:B358,C9:C358,C5)</f>
+        <v>Figure@40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="str" cm="1">
+        <f t="array" ref="D6">_xll.show_matplotlib_ctp(D5,C6)</f>
+        <v>Figure@41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
@@ -634,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>0</v>
       </c>
@@ -643,7 +669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <f>B9+0.05</f>
         <v>0.05</v>
@@ -653,7 +679,7 @@
         <v>7.2798500044011921E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <f t="shared" ref="B11:B74" si="1">B10+0.05</f>
         <v>0.1</v>
@@ -663,7 +689,7 @@
         <v>0.30260644336050269</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
@@ -673,7 +699,7 @@
         <v>0.5748347242212053</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <f t="shared" si="1"/>
         <v>0.2</v>
@@ -683,7 +709,7 @@
         <v>0.63218922317423532</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -693,7 +719,7 @@
         <v>0.42798728108473139</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <f t="shared" si="1"/>
         <v>0.3</v>
@@ -703,7 +729,7 @@
         <v>0.20141283447755312</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
         <f t="shared" si="1"/>
         <v>0.35</v>

</xml_diff>